<commit_message>
Planeacion: Herramientas de administracion de riesgos...Se modificaron los campos de prioridad, status, y fecha de modificacion en la pestaña Detalle de riesgo y se agrego la localizacion del documento en la pestaña Identificacion
</commit_message>
<xml_diff>
--- a/Documentacion/2 Planeacion/PP_HER_v1_Herramienta para la Administración de Riesgos MEPPP.xlsx
+++ b/Documentacion/2 Planeacion/PP_HER_v1_Herramienta para la Administración de Riesgos MEPPP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIOVANNI\Desktop\04_MEPPP\Anexos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIOVANNI\OneDrive\Riesgos MEPPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{71E2F084-0E2E-4400-97F1-19112F181867}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{91046F40-2F30-4A1A-90A9-831F920F9DA6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identificacion" sheetId="9" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2437" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2445" uniqueCount="389">
   <si>
     <t xml:space="preserve">El informe del resumen de los riesgos sintetiza el estado total de los riesgos en el proyecto.  </t>
   </si>
@@ -1122,9 +1122,6 @@
     <t>Descripción del Cambio</t>
   </si>
   <si>
-    <t>Recien creado</t>
-  </si>
-  <si>
     <t>Herramienta de administracion de riesgos</t>
   </si>
   <si>
@@ -1149,12 +1146,6 @@
     <t>Giovanni Misael Alfaro Sánchez</t>
   </si>
   <si>
-    <t>One Drive/Riesgos MEPPP</t>
-  </si>
-  <si>
-    <t>GMAS</t>
-  </si>
-  <si>
     <t>Proyecto:  MEPPP</t>
   </si>
   <si>
@@ -1579,6 +1570,27 @@
   </si>
   <si>
     <t>Evitar comportamientos que atenten contra su integridad.</t>
+  </si>
+  <si>
+    <t>14/Junio/2018- Se notifico al equipo de desarrollo de las medidas de mitigación.</t>
+  </si>
+  <si>
+    <t>Recien creado.</t>
+  </si>
+  <si>
+    <t>Modificación de prioridad de riesgos y estatus.</t>
+  </si>
+  <si>
+    <t>Jonathan Jair Alfaro Sanchez</t>
+  </si>
+  <si>
+    <t>Mary Carmen Crescencio Bernal</t>
+  </si>
+  <si>
+    <t>Miguel Ángel Mandujano Barragán</t>
+  </si>
+  <si>
+    <t>https://github.com/JOMIMAN-Solutions/MEPPP/tree/master/Documentacion/2%20Planeacion</t>
   </si>
 </sst>
 </file>
@@ -1588,7 +1600,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1708,6 +1720,18 @@
       <color indexed="9"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="12">
@@ -2138,11 +2162,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="229">
+  <cellXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2699,9 +2724,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2759,6 +2781,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2771,8 +2823,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_RM_Risks" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
@@ -3424,7 +3480,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -3554,7 +3610,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -3678,10 +3734,10 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
@@ -3940,10 +3996,10 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -4000,14 +4056,8 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect r="4683" b="5927"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4052,14 +4102,8 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="email">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect l="39583" t="26041" r="19011" b="14931"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6587,10 +6631,10 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="email">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -6941,8 +6985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6954,31 +6998,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="228"/>
-      <c r="B2" s="228"/>
+      <c r="A2" s="237"/>
+      <c r="B2" s="237"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="228"/>
-      <c r="B3" s="228"/>
+      <c r="A3" s="237"/>
+      <c r="B3" s="237"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="228"/>
-      <c r="B4" s="228"/>
+      <c r="A4" s="237"/>
+      <c r="B4" s="237"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="228"/>
-      <c r="B5" s="228"/>
+      <c r="A5" s="237"/>
+      <c r="B5" s="237"/>
     </row>
     <row r="7" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A7" s="193" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="194"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="206" t="s">
+      <c r="A9" s="205" t="s">
         <v>218</v>
       </c>
       <c r="B9" s="195" t="s">
@@ -6988,17 +7032,17 @@
       <c r="D9" s="195"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="206" t="s">
+      <c r="A10" s="205" t="s">
         <v>220</v>
       </c>
       <c r="B10" s="204" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C10" s="195"/>
       <c r="D10" s="195"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="206" t="s">
+      <c r="A11" s="205" t="s">
         <v>221</v>
       </c>
       <c r="B11" s="196">
@@ -7008,21 +7052,21 @@
       <c r="D11" s="195"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="206" t="s">
+      <c r="A12" s="205" t="s">
         <v>222</v>
       </c>
-      <c r="B12" s="205" t="s">
-        <v>240</v>
+      <c r="B12" s="227" t="s">
+        <v>239</v>
       </c>
       <c r="C12" s="195"/>
       <c r="D12" s="195"/>
     </row>
-    <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="206" t="s">
+    <row r="13" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="205" t="s">
         <v>223</v>
       </c>
-      <c r="B13" s="205" t="s">
-        <v>241</v>
+      <c r="B13" s="238" t="s">
+        <v>388</v>
       </c>
       <c r="C13" s="195"/>
       <c r="D13" s="195"/>
@@ -7034,128 +7078,163 @@
       <c r="D14" s="195"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="225" t="s">
+      <c r="A15" s="234" t="s">
         <v>224</v>
       </c>
-      <c r="B15" s="226"/>
+      <c r="B15" s="235"/>
       <c r="C15" s="197"/>
       <c r="D15" s="197"/>
       <c r="E15" s="198"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="206" t="s">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="205" t="s">
         <v>225</v>
       </c>
-      <c r="B16" s="206" t="s">
+      <c r="B16" s="205" t="s">
         <v>226</v>
       </c>
       <c r="C16" s="195"/>
-      <c r="D16" s="195"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="199"/>
-      <c r="B17" s="199"/>
+      <c r="D16" s="230"/>
+    </row>
+    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="224" t="s">
+        <v>239</v>
+      </c>
+      <c r="B17" s="228">
+        <v>43265</v>
+      </c>
       <c r="C17" s="195"/>
-      <c r="D17" s="195"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="230"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="199"/>
       <c r="B18" s="199"/>
       <c r="C18" s="195"/>
-      <c r="D18" s="195"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="230"/>
+    </row>
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="199"/>
       <c r="B19" s="199"/>
       <c r="C19" s="195"/>
-      <c r="D19" s="195"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="230"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="195"/>
       <c r="B20" s="195"/>
       <c r="C20" s="195"/>
       <c r="D20" s="195"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="225" t="s">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="234" t="s">
         <v>227</v>
       </c>
-      <c r="B21" s="226"/>
+      <c r="B21" s="235"/>
       <c r="C21" s="195"/>
       <c r="D21" s="195"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="206" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="205" t="s">
         <v>225</v>
       </c>
-      <c r="B22" s="206" t="s">
+      <c r="B22" s="205" t="s">
         <v>228</v>
       </c>
       <c r="C22" s="195"/>
       <c r="D22" s="195"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="199"/>
-      <c r="B23" s="199"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="199" t="s">
+        <v>385</v>
+      </c>
+      <c r="B23" s="225">
+        <v>43265</v>
+      </c>
       <c r="C23" s="195"/>
       <c r="D23" s="195"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="199"/>
-      <c r="B24" s="199"/>
+    <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="199" t="s">
+        <v>386</v>
+      </c>
+      <c r="B24" s="225">
+        <v>43265</v>
+      </c>
       <c r="C24" s="195"/>
       <c r="D24" s="195"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="199"/>
-      <c r="B25" s="199"/>
+    <row r="25" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="231" t="s">
+        <v>387</v>
+      </c>
+      <c r="B25" s="225">
+        <v>43265</v>
+      </c>
       <c r="C25" s="195"/>
       <c r="D25" s="195"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="195"/>
       <c r="B26" s="195"/>
       <c r="C26" s="195"/>
       <c r="D26" s="195"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="225" t="s">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="234" t="s">
         <v>229</v>
       </c>
-      <c r="B27" s="227"/>
-      <c r="C27" s="227"/>
-      <c r="D27" s="226"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="206" t="s">
+      <c r="B27" s="236"/>
+      <c r="C27" s="236"/>
+      <c r="D27" s="235"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="205" t="s">
         <v>218</v>
       </c>
-      <c r="B28" s="207" t="s">
+      <c r="B28" s="206" t="s">
         <v>221</v>
       </c>
-      <c r="C28" s="207" t="s">
+      <c r="C28" s="206" t="s">
         <v>230</v>
       </c>
-      <c r="D28" s="207" t="s">
+      <c r="D28" s="206" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="199">
+    <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="224">
         <v>1</v>
       </c>
-      <c r="B29" s="196">
+      <c r="B29" s="225">
         <v>39613</v>
       </c>
-      <c r="C29" s="195" t="s">
-        <v>242</v>
-      </c>
-      <c r="D29" s="199" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="199" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:4" s="199" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="C29" s="226" t="s">
+        <v>239</v>
+      </c>
+      <c r="D29" s="224" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="199" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="224">
+        <v>2</v>
+      </c>
+      <c r="B30" s="225">
+        <v>39627</v>
+      </c>
+      <c r="C30" s="224" t="s">
+        <v>239</v>
+      </c>
+      <c r="D30" s="224" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="199" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="233"/>
+      <c r="B31" s="233"/>
+      <c r="C31" s="233"/>
+      <c r="D31" s="233"/>
+      <c r="E31" s="232"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A15:B15"/>
@@ -7164,9 +7243,13 @@
     <mergeCell ref="A2:B5"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{2C5A0290-DB1B-4BBE-AA53-06E4B82A3567}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -7177,8 +7260,8 @@
   </sheetPr>
   <dimension ref="A1:K147"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8042,9 +8125,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:AB783"/>
   <sheetViews>
-    <sheetView topLeftCell="A548" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F550" sqref="F550"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8070,8 +8151,8 @@
     <row r="2" spans="2:28" s="100" customFormat="1" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="188"/>
       <c r="C2" s="99"/>
-      <c r="D2" s="212" t="s">
-        <v>243</v>
+      <c r="D2" s="211" t="s">
+        <v>240</v>
       </c>
       <c r="E2" s="185" t="s">
         <v>81</v>
@@ -8090,17 +8171,17 @@
       <c r="B3" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="215" t="s">
-        <v>269</v>
+      <c r="C3" s="214" t="s">
+        <v>266</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E3" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F3" s="167" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="I3" s="137" t="s">
         <v>92</v>
@@ -8113,8 +8194,8 @@
       <c r="B4" s="189" t="s">
         <v>215</v>
       </c>
-      <c r="C4" s="214" t="s">
-        <v>248</v>
+      <c r="C4" s="213" t="s">
+        <v>245</v>
       </c>
       <c r="D4" s="191"/>
       <c r="E4" s="21"/>
@@ -8136,7 +8217,7 @@
         <v>135</v>
       </c>
       <c r="F5" s="112">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I5" s="137" t="s">
         <v>92</v>
@@ -8149,8 +8230,8 @@
       <c r="B6" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="209" t="s">
-        <v>347</v>
+      <c r="C6" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>126</v>
@@ -8159,7 +8240,7 @@
         <v>56</v>
       </c>
       <c r="F6" s="133" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="I6" s="137" t="s">
         <v>92</v>
@@ -8172,8 +8253,8 @@
       <c r="B7" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="210" t="s">
-        <v>347</v>
+      <c r="C7" s="209" t="s">
+        <v>344</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="16" t="s">
@@ -8218,7 +8299,7 @@
         <v>50</v>
       </c>
       <c r="C9" s="132" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>96</v>
@@ -8226,7 +8307,7 @@
       <c r="E9" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="211">
+      <c r="F9" s="210">
         <v>43265</v>
       </c>
       <c r="I9" s="137" t="s">
@@ -8241,7 +8322,7 @@
         <v>57</v>
       </c>
       <c r="C10" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>99</v>
@@ -8250,7 +8331,7 @@
         <v>62</v>
       </c>
       <c r="F10" s="134">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I10" s="137" t="s">
         <v>92</v>
@@ -8277,8 +8358,8 @@
       <c r="C12" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="213" t="s">
-        <v>247</v>
+      <c r="D12" s="212" t="s">
+        <v>244</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="19"/>
@@ -8307,8 +8388,8 @@
       <c r="C14" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="213" t="s">
-        <v>378</v>
+      <c r="D14" s="212" t="s">
+        <v>375</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="19"/>
@@ -8418,7 +8499,7 @@
       <c r="B22" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="208" t="s">
+      <c r="C22" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D22" s="48" t="s">
@@ -8438,19 +8519,19 @@
       </c>
     </row>
     <row r="23" spans="2:28" ht="51" x14ac:dyDescent="0.2">
-      <c r="B23" s="220" t="s">
-        <v>347</v>
-      </c>
-      <c r="C23" s="221">
+      <c r="B23" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C23" s="220">
         <v>1</v>
       </c>
-      <c r="D23" s="219" t="s">
-        <v>337</v>
-      </c>
-      <c r="E23" s="222">
+      <c r="D23" s="218" t="s">
+        <v>334</v>
+      </c>
+      <c r="E23" s="221">
         <v>43265</v>
       </c>
-      <c r="F23" s="223">
+      <c r="F23" s="222">
         <v>43265</v>
       </c>
       <c r="I23" s="137" t="s">
@@ -8538,17 +8619,17 @@
       <c r="B30" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C30" s="215" t="s">
-        <v>270</v>
+      <c r="C30" s="214" t="s">
+        <v>267</v>
       </c>
       <c r="D30" s="165" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E30" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F30" s="167" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="I30" s="137" t="s">
         <v>92</v>
@@ -8582,7 +8663,7 @@
         <v>135</v>
       </c>
       <c r="F32" s="112">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I32" s="137" t="s">
         <v>92</v>
@@ -8595,8 +8676,8 @@
       <c r="B33" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C33" s="209" t="s">
-        <v>347</v>
+      <c r="C33" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>126</v>
@@ -8605,7 +8686,7 @@
         <v>56</v>
       </c>
       <c r="F33" s="133" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="I33" s="137" t="s">
         <v>92</v>
@@ -8618,8 +8699,8 @@
       <c r="B34" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="209" t="s">
-        <v>347</v>
+      <c r="C34" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="16" t="s">
@@ -8653,7 +8734,7 @@
         <v>44</v>
       </c>
       <c r="C35" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D35" s="49" t="str">
         <f>IF(C35="","WARNING - Please enter a Probability.","")</f>
@@ -8677,7 +8758,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="132" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>96</v>
@@ -8685,7 +8766,7 @@
       <c r="E36" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F36" s="211">
+      <c r="F36" s="210">
         <v>43265</v>
       </c>
       <c r="I36" s="137" t="s">
@@ -8700,7 +8781,7 @@
         <v>57</v>
       </c>
       <c r="C37" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>99</v>
@@ -8709,7 +8790,7 @@
         <v>62</v>
       </c>
       <c r="F37" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I37" s="137" t="s">
         <v>92</v>
@@ -8736,8 +8817,8 @@
       <c r="C39" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D39" s="217" t="s">
-        <v>298</v>
+      <c r="D39" s="216" t="s">
+        <v>295</v>
       </c>
       <c r="E39" s="18"/>
       <c r="F39" s="19"/>
@@ -8767,7 +8848,7 @@
         <v>90</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E41" s="18"/>
       <c r="F41" s="19"/>
@@ -8877,7 +8958,7 @@
       <c r="B49" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C49" s="208" t="s">
+      <c r="C49" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D49" s="48" t="s">
@@ -8897,19 +8978,19 @@
       </c>
     </row>
     <row r="50" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B50" s="220" t="s">
-        <v>347</v>
-      </c>
-      <c r="C50" s="221">
+      <c r="B50" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C50" s="220">
         <v>1</v>
       </c>
       <c r="D50" s="172" t="s">
-        <v>339</v>
-      </c>
-      <c r="E50" s="222">
+        <v>336</v>
+      </c>
+      <c r="E50" s="221">
         <v>43265</v>
       </c>
-      <c r="F50" s="223">
+      <c r="F50" s="222">
         <v>43265</v>
       </c>
       <c r="I50" s="137" t="s">
@@ -8920,19 +9001,19 @@
       </c>
     </row>
     <row r="51" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B51" s="224" t="s">
-        <v>347</v>
-      </c>
-      <c r="C51" s="221">
+      <c r="B51" s="223" t="s">
+        <v>344</v>
+      </c>
+      <c r="C51" s="220">
         <v>2</v>
       </c>
       <c r="D51" s="172" t="s">
-        <v>338</v>
-      </c>
-      <c r="E51" s="222">
+        <v>335</v>
+      </c>
+      <c r="E51" s="221">
         <v>43266</v>
       </c>
-      <c r="F51" s="223">
+      <c r="F51" s="222">
         <v>43266</v>
       </c>
       <c r="I51" s="137" t="s">
@@ -8943,19 +9024,19 @@
       </c>
     </row>
     <row r="52" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B52" s="224" t="s">
-        <v>347</v>
-      </c>
-      <c r="C52" s="221">
+      <c r="B52" s="223" t="s">
+        <v>344</v>
+      </c>
+      <c r="C52" s="220">
         <v>3</v>
       </c>
       <c r="D52" s="172" t="s">
-        <v>340</v>
-      </c>
-      <c r="E52" s="222">
+        <v>337</v>
+      </c>
+      <c r="E52" s="221">
         <v>43267</v>
       </c>
-      <c r="F52" s="223">
+      <c r="F52" s="222">
         <v>43267</v>
       </c>
       <c r="I52" s="137" t="s">
@@ -9024,17 +9105,17 @@
       <c r="B56" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C56" s="215" t="s">
-        <v>271</v>
+      <c r="C56" s="214" t="s">
+        <v>268</v>
       </c>
       <c r="D56" s="165" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E56" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F56" s="167" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I56" s="137" t="s">
         <v>92</v>
@@ -9070,7 +9151,7 @@
       <c r="B58" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C58" s="209">
+      <c r="C58" s="208">
         <v>43265</v>
       </c>
       <c r="D58" s="15" t="str">
@@ -9081,7 +9162,7 @@
         <v>135</v>
       </c>
       <c r="F58" s="112">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I58" s="137" t="s">
         <v>92</v>
@@ -9094,8 +9175,8 @@
       <c r="B59" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C59" s="209" t="s">
-        <v>347</v>
+      <c r="C59" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D59" s="15" t="s">
         <v>126</v>
@@ -9104,7 +9185,7 @@
         <v>56</v>
       </c>
       <c r="F59" s="133" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I59" s="137" t="s">
         <v>92</v>
@@ -9117,8 +9198,8 @@
       <c r="B60" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C60" s="209" t="s">
-        <v>347</v>
+      <c r="C60" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D60" s="18"/>
       <c r="E60" s="16" t="s">
@@ -9139,7 +9220,7 @@
         <v>44</v>
       </c>
       <c r="C61" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D61" s="49" t="str">
         <f>IF(C61="","WARNING - Please enter a Probability.","")</f>
@@ -9163,7 +9244,7 @@
         <v>50</v>
       </c>
       <c r="C62" s="132" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D62" s="15" t="s">
         <v>96</v>
@@ -9171,7 +9252,7 @@
       <c r="E62" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F62" s="211">
+      <c r="F62" s="210">
         <v>43265</v>
       </c>
       <c r="I62" s="137" t="s">
@@ -9194,8 +9275,8 @@
       <c r="E63" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="F63" s="216">
-        <v>43265</v>
+      <c r="F63" s="215">
+        <v>43279</v>
       </c>
       <c r="I63" s="137" t="s">
         <v>92</v>
@@ -9222,8 +9303,8 @@
       <c r="C65" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D65" s="217" t="s">
-        <v>300</v>
+      <c r="D65" s="216" t="s">
+        <v>297</v>
       </c>
       <c r="E65" s="18"/>
       <c r="F65" s="19"/>
@@ -9253,7 +9334,7 @@
         <v>90</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E67" s="18"/>
       <c r="F67" s="19"/>
@@ -9363,7 +9444,7 @@
       <c r="B75" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C75" s="208" t="s">
+      <c r="C75" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D75" s="48" t="s">
@@ -9383,19 +9464,19 @@
       </c>
     </row>
     <row r="76" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B76" s="220" t="s">
+      <c r="B76" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C76" s="220">
+        <v>1</v>
+      </c>
+      <c r="D76" s="22" t="s">
         <v>347</v>
       </c>
-      <c r="C76" s="221">
-        <v>1</v>
-      </c>
-      <c r="D76" s="22" t="s">
-        <v>350</v>
-      </c>
-      <c r="E76" s="222">
+      <c r="E76" s="221">
         <v>43265</v>
       </c>
-      <c r="F76" s="223">
+      <c r="F76" s="222">
         <v>43265</v>
       </c>
       <c r="I76" s="137" t="s">
@@ -9406,19 +9487,19 @@
       </c>
     </row>
     <row r="77" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B77" s="220" t="s">
-        <v>347</v>
-      </c>
-      <c r="C77" s="221">
+      <c r="B77" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C77" s="220">
         <v>2</v>
       </c>
       <c r="D77" s="22" t="s">
-        <v>351</v>
-      </c>
-      <c r="E77" s="222">
+        <v>348</v>
+      </c>
+      <c r="E77" s="221">
         <v>43266</v>
       </c>
-      <c r="F77" s="223">
+      <c r="F77" s="222">
         <v>43266</v>
       </c>
       <c r="I77" s="137" t="s">
@@ -9484,17 +9565,17 @@
       <c r="B82" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C82" s="215" t="s">
-        <v>272</v>
+      <c r="C82" s="214" t="s">
+        <v>269</v>
       </c>
       <c r="D82" s="165" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E82" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F82" s="167" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="I82" s="137" t="s">
         <v>92</v>
@@ -9517,7 +9598,7 @@
       <c r="B84" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C84" s="209">
+      <c r="C84" s="208">
         <v>43265</v>
       </c>
       <c r="D84" s="15" t="str">
@@ -9528,7 +9609,7 @@
         <v>135</v>
       </c>
       <c r="F84" s="112">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I84" s="137" t="s">
         <v>92</v>
@@ -9541,8 +9622,8 @@
       <c r="B85" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C85" s="209" t="s">
-        <v>347</v>
+      <c r="C85" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D85" s="15" t="s">
         <v>126</v>
@@ -9551,7 +9632,7 @@
         <v>56</v>
       </c>
       <c r="F85" s="133" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I85" s="137" t="s">
         <v>92</v>
@@ -9564,8 +9645,8 @@
       <c r="B86" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C86" s="209" t="s">
-        <v>347</v>
+      <c r="C86" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D86" s="18"/>
       <c r="E86" s="16" t="s">
@@ -9610,7 +9691,7 @@
         <v>50</v>
       </c>
       <c r="C88" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D88" s="15" t="s">
         <v>96</v>
@@ -9618,7 +9699,7 @@
       <c r="E88" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F88" s="211">
+      <c r="F88" s="210">
         <v>43265</v>
       </c>
       <c r="I88" s="137" t="s">
@@ -9641,8 +9722,8 @@
       <c r="E89" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="F89" s="216">
-        <v>43265</v>
+      <c r="F89" s="229">
+        <v>43279</v>
       </c>
       <c r="I89" s="137" t="s">
         <v>92</v>
@@ -9669,8 +9750,8 @@
       <c r="C91" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D91" s="217" t="s">
-        <v>302</v>
+      <c r="D91" s="216" t="s">
+        <v>299</v>
       </c>
       <c r="E91" s="18"/>
       <c r="F91" s="19"/>
@@ -9700,7 +9781,7 @@
         <v>90</v>
       </c>
       <c r="D93" s="22" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E93" s="18"/>
       <c r="F93" s="19"/>
@@ -9810,7 +9891,7 @@
       <c r="B101" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C101" s="208" t="s">
+      <c r="C101" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D101" s="48" t="s">
@@ -9830,19 +9911,19 @@
       </c>
     </row>
     <row r="102" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B102" s="220" t="s">
-        <v>347</v>
-      </c>
-      <c r="C102" s="221">
+      <c r="B102" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C102" s="220">
         <v>1</v>
       </c>
       <c r="D102" s="22" t="s">
-        <v>352</v>
-      </c>
-      <c r="E102" s="222">
+        <v>349</v>
+      </c>
+      <c r="E102" s="221">
         <v>43265</v>
       </c>
-      <c r="F102" s="223">
+      <c r="F102" s="222">
         <v>43265</v>
       </c>
       <c r="I102" s="137" t="s">
@@ -9853,19 +9934,19 @@
       </c>
     </row>
     <row r="103" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B103" s="220" t="s">
-        <v>347</v>
-      </c>
-      <c r="C103" s="221">
+      <c r="B103" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C103" s="220">
         <v>2</v>
       </c>
       <c r="D103" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="E103" s="222">
+        <v>350</v>
+      </c>
+      <c r="E103" s="221">
         <v>43266</v>
       </c>
-      <c r="F103" s="223">
+      <c r="F103" s="222">
         <v>43266</v>
       </c>
       <c r="I103" s="137" t="s">
@@ -9931,17 +10012,17 @@
       <c r="B108" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C108" s="215" t="s">
-        <v>273</v>
+      <c r="C108" s="214" t="s">
+        <v>270</v>
       </c>
       <c r="D108" s="165" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E108" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F108" s="167" t="s">
-        <v>104</v>
+        <v>377</v>
       </c>
       <c r="I108" s="137" t="s">
         <v>92</v>
@@ -9975,7 +10056,7 @@
         <v>135</v>
       </c>
       <c r="F110" s="112">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I110" s="137" t="s">
         <v>92</v>
@@ -9988,8 +10069,8 @@
       <c r="B111" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C111" s="209" t="s">
-        <v>347</v>
+      <c r="C111" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D111" s="15" t="s">
         <v>126</v>
@@ -10011,8 +10092,8 @@
       <c r="B112" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C112" s="209" t="s">
-        <v>336</v>
+      <c r="C112" s="208" t="s">
+        <v>333</v>
       </c>
       <c r="D112" s="18"/>
       <c r="E112" s="16" t="s">
@@ -10057,7 +10138,7 @@
         <v>50</v>
       </c>
       <c r="C114" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D114" s="15" t="s">
         <v>96</v>
@@ -10080,7 +10161,7 @@
         <v>57</v>
       </c>
       <c r="C115" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D115" s="15" t="s">
         <v>99</v>
@@ -10089,7 +10170,7 @@
         <v>62</v>
       </c>
       <c r="F115" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I115" s="137" t="s">
         <v>92</v>
@@ -10116,8 +10197,8 @@
       <c r="C117" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D117" s="217" t="s">
-        <v>304</v>
+      <c r="D117" s="216" t="s">
+        <v>301</v>
       </c>
       <c r="E117" s="18"/>
       <c r="F117" s="19"/>
@@ -10147,7 +10228,7 @@
         <v>90</v>
       </c>
       <c r="D119" s="22" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E119" s="18"/>
       <c r="F119" s="19"/>
@@ -10257,7 +10338,7 @@
       <c r="B127" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C127" s="208" t="s">
+      <c r="C127" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D127" s="48" t="s">
@@ -10277,19 +10358,19 @@
       </c>
     </row>
     <row r="128" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B128" s="220" t="s">
-        <v>336</v>
-      </c>
-      <c r="C128" s="221">
+      <c r="B128" s="219" t="s">
+        <v>333</v>
+      </c>
+      <c r="C128" s="220">
         <v>1</v>
       </c>
       <c r="D128" s="22" t="s">
-        <v>354</v>
-      </c>
-      <c r="E128" s="222">
+        <v>351</v>
+      </c>
+      <c r="E128" s="221">
         <v>43265</v>
       </c>
-      <c r="F128" s="223">
+      <c r="F128" s="222">
         <v>43265</v>
       </c>
       <c r="I128" s="137" t="s">
@@ -10300,19 +10381,19 @@
       </c>
     </row>
     <row r="129" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B129" s="220" t="s">
-        <v>347</v>
-      </c>
-      <c r="C129" s="221">
+      <c r="B129" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C129" s="220">
         <v>2</v>
       </c>
       <c r="D129" s="22" t="s">
-        <v>355</v>
-      </c>
-      <c r="E129" s="222">
+        <v>352</v>
+      </c>
+      <c r="E129" s="221">
         <v>43266</v>
       </c>
-      <c r="F129" s="223">
+      <c r="F129" s="222">
         <v>43266</v>
       </c>
       <c r="I129" s="137" t="s">
@@ -10378,11 +10459,11 @@
       <c r="B134" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C134" s="215" t="s">
-        <v>274</v>
+      <c r="C134" s="214" t="s">
+        <v>271</v>
       </c>
       <c r="D134" s="165" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E134" s="166" t="s">
         <v>51</v>
@@ -10422,7 +10503,7 @@
         <v>135</v>
       </c>
       <c r="F136" s="112">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I136" s="137" t="s">
         <v>92</v>
@@ -10435,8 +10516,8 @@
       <c r="B137" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C137" s="209" t="s">
-        <v>347</v>
+      <c r="C137" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D137" s="15" t="s">
         <v>126</v>
@@ -10445,7 +10526,7 @@
         <v>56</v>
       </c>
       <c r="F137" s="133" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I137" s="137" t="s">
         <v>92</v>
@@ -10458,8 +10539,8 @@
       <c r="B138" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C138" s="209" t="s">
-        <v>347</v>
+      <c r="C138" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D138" s="18"/>
       <c r="E138" s="16" t="s">
@@ -10504,7 +10585,7 @@
         <v>50</v>
       </c>
       <c r="C140" s="132" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D140" s="15" t="s">
         <v>96</v>
@@ -10527,7 +10608,7 @@
         <v>57</v>
       </c>
       <c r="C141" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D141" s="15" t="s">
         <v>99</v>
@@ -10536,7 +10617,7 @@
         <v>62</v>
       </c>
       <c r="F141" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I141" s="137" t="s">
         <v>92</v>
@@ -10563,8 +10644,8 @@
       <c r="C143" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D143" s="217" t="s">
-        <v>306</v>
+      <c r="D143" s="216" t="s">
+        <v>303</v>
       </c>
       <c r="E143" s="18"/>
       <c r="F143" s="19"/>
@@ -10594,7 +10675,7 @@
         <v>90</v>
       </c>
       <c r="D145" s="22" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E145" s="18"/>
       <c r="F145" s="19"/>
@@ -10704,7 +10785,7 @@
       <c r="B153" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C153" s="208" t="s">
+      <c r="C153" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D153" s="48" t="s">
@@ -10724,19 +10805,19 @@
       </c>
     </row>
     <row r="154" spans="2:28" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B154" s="220" t="s">
-        <v>347</v>
-      </c>
-      <c r="C154" s="221">
+      <c r="B154" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C154" s="220">
         <v>1</v>
       </c>
       <c r="D154" s="172" t="s">
-        <v>341</v>
-      </c>
-      <c r="E154" s="222">
+        <v>338</v>
+      </c>
+      <c r="E154" s="221">
         <v>43265</v>
       </c>
-      <c r="F154" s="223">
+      <c r="F154" s="222">
         <v>43265</v>
       </c>
       <c r="I154" s="137" t="s">
@@ -10812,17 +10893,17 @@
       <c r="B160" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C160" s="215" t="s">
-        <v>275</v>
+      <c r="C160" s="214" t="s">
+        <v>272</v>
       </c>
       <c r="D160" s="165" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E160" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F160" s="167" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="I160" s="137" t="s">
         <v>93</v>
@@ -10856,7 +10937,7 @@
         <v>135</v>
       </c>
       <c r="F162" s="112">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="I162" s="137" t="s">
         <v>93</v>
@@ -10869,8 +10950,8 @@
       <c r="B163" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C163" s="209" t="s">
-        <v>347</v>
+      <c r="C163" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D163" s="15" t="s">
         <v>126</v>
@@ -10879,7 +10960,7 @@
         <v>56</v>
       </c>
       <c r="F163" s="133" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="I163" s="137" t="s">
         <v>93</v>
@@ -10892,8 +10973,8 @@
       <c r="B164" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C164" s="209" t="s">
-        <v>347</v>
+      <c r="C164" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D164" s="18"/>
       <c r="E164" s="16" t="s">
@@ -10914,7 +10995,7 @@
         <v>44</v>
       </c>
       <c r="C165" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D165" s="49" t="str">
         <f>IF(C165="","WARNING - Please enter a Probability.","")</f>
@@ -10938,7 +11019,7 @@
         <v>50</v>
       </c>
       <c r="C166" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D166" s="15" t="s">
         <v>96</v>
@@ -10961,7 +11042,7 @@
         <v>57</v>
       </c>
       <c r="C167" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D167" s="15" t="s">
         <v>99</v>
@@ -10970,7 +11051,7 @@
         <v>62</v>
       </c>
       <c r="F167" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I167" s="137" t="s">
         <v>93</v>
@@ -10997,8 +11078,8 @@
       <c r="C169" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D169" s="217" t="s">
-        <v>308</v>
+      <c r="D169" s="216" t="s">
+        <v>305</v>
       </c>
       <c r="E169" s="18"/>
       <c r="F169" s="19"/>
@@ -11028,7 +11109,7 @@
         <v>90</v>
       </c>
       <c r="D171" s="22" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E171" s="18"/>
       <c r="F171" s="19"/>
@@ -11138,7 +11219,7 @@
       <c r="B179" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C179" s="208" t="s">
+      <c r="C179" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D179" s="48" t="s">
@@ -11158,19 +11239,19 @@
       </c>
     </row>
     <row r="180" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B180" s="220" t="s">
-        <v>347</v>
-      </c>
-      <c r="C180" s="221">
+      <c r="B180" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C180" s="220">
         <v>1</v>
       </c>
       <c r="D180" s="22" t="s">
-        <v>356</v>
-      </c>
-      <c r="E180" s="222">
+        <v>353</v>
+      </c>
+      <c r="E180" s="221">
         <v>43265</v>
       </c>
-      <c r="F180" s="223">
+      <c r="F180" s="222">
         <v>43265</v>
       </c>
       <c r="I180" s="137" t="s">
@@ -11181,19 +11262,19 @@
       </c>
     </row>
     <row r="181" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B181" s="220" t="s">
-        <v>347</v>
-      </c>
-      <c r="C181" s="221">
+      <c r="B181" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C181" s="220">
         <v>2</v>
       </c>
       <c r="D181" s="22" t="s">
-        <v>357</v>
-      </c>
-      <c r="E181" s="222">
+        <v>354</v>
+      </c>
+      <c r="E181" s="221">
         <v>43266</v>
       </c>
-      <c r="F181" s="223">
+      <c r="F181" s="222">
         <v>43266</v>
       </c>
       <c r="I181" s="137" t="s">
@@ -11256,17 +11337,17 @@
       <c r="B186" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C186" s="215" t="s">
-        <v>276</v>
+      <c r="C186" s="214" t="s">
+        <v>273</v>
       </c>
       <c r="D186" s="165" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E186" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F186" s="167" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="I186" s="137" t="s">
         <v>93</v>
@@ -11313,8 +11394,8 @@
       <c r="B189" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C189" s="209" t="s">
-        <v>347</v>
+      <c r="C189" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D189" s="15" t="s">
         <v>126</v>
@@ -11323,7 +11404,7 @@
         <v>56</v>
       </c>
       <c r="F189" s="133" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I189" s="137" t="s">
         <v>93</v>
@@ -11336,8 +11417,8 @@
       <c r="B190" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C190" s="209" t="s">
-        <v>336</v>
+      <c r="C190" s="208" t="s">
+        <v>333</v>
       </c>
       <c r="D190" s="18"/>
       <c r="E190" s="16" t="s">
@@ -11358,7 +11439,7 @@
         <v>44</v>
       </c>
       <c r="C191" s="132" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D191" s="49" t="str">
         <f>IF(C191="","WARNING - Please enter a Probability.","")</f>
@@ -11382,7 +11463,7 @@
         <v>50</v>
       </c>
       <c r="C192" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D192" s="15" t="s">
         <v>96</v>
@@ -11405,7 +11486,7 @@
         <v>57</v>
       </c>
       <c r="C193" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D193" s="15" t="s">
         <v>99</v>
@@ -11414,7 +11495,7 @@
         <v>62</v>
       </c>
       <c r="F193" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I193" s="137" t="s">
         <v>93</v>
@@ -11441,8 +11522,8 @@
       <c r="C195" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D195" s="217" t="s">
-        <v>383</v>
+      <c r="D195" s="216" t="s">
+        <v>380</v>
       </c>
       <c r="E195" s="18"/>
       <c r="F195" s="19"/>
@@ -11472,7 +11553,7 @@
         <v>90</v>
       </c>
       <c r="D197" s="22" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E197" s="18"/>
       <c r="F197" s="19"/>
@@ -11582,7 +11663,7 @@
       <c r="B205" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C205" s="208" t="s">
+      <c r="C205" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D205" s="48" t="s">
@@ -11602,19 +11683,19 @@
       </c>
     </row>
     <row r="206" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B206" s="220" t="s">
-        <v>347</v>
-      </c>
-      <c r="C206" s="221">
+      <c r="B206" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C206" s="220">
         <v>1</v>
       </c>
       <c r="D206" s="22" t="s">
-        <v>358</v>
-      </c>
-      <c r="E206" s="222">
+        <v>355</v>
+      </c>
+      <c r="E206" s="221">
         <v>43265</v>
       </c>
-      <c r="F206" s="223">
+      <c r="F206" s="222">
         <v>43265</v>
       </c>
       <c r="I206" s="137" t="s">
@@ -11690,17 +11771,17 @@
       <c r="B212" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C212" s="215" t="s">
-        <v>277</v>
+      <c r="C212" s="214" t="s">
+        <v>274</v>
       </c>
       <c r="D212" s="165" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E212" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F212" s="167" t="s">
-        <v>104</v>
+        <v>377</v>
       </c>
       <c r="I212" s="137" t="s">
         <v>93</v>
@@ -11734,7 +11815,7 @@
         <v>135</v>
       </c>
       <c r="F214" s="112">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I214" s="137" t="s">
         <v>93</v>
@@ -11747,8 +11828,8 @@
       <c r="B215" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C215" s="209" t="s">
-        <v>347</v>
+      <c r="C215" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D215" s="15" t="s">
         <v>126</v>
@@ -11757,7 +11838,7 @@
         <v>56</v>
       </c>
       <c r="F215" s="133" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="I215" s="137" t="s">
         <v>93</v>
@@ -11770,8 +11851,8 @@
       <c r="B216" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C216" s="209" t="s">
-        <v>336</v>
+      <c r="C216" s="208" t="s">
+        <v>333</v>
       </c>
       <c r="D216" s="18"/>
       <c r="E216" s="16" t="s">
@@ -11792,7 +11873,7 @@
         <v>44</v>
       </c>
       <c r="C217" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D217" s="49" t="str">
         <f>IF(C217="","WARNING - Please enter a Probability.","")</f>
@@ -11839,7 +11920,7 @@
         <v>57</v>
       </c>
       <c r="C219" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D219" s="15" t="s">
         <v>99</v>
@@ -11848,7 +11929,7 @@
         <v>62</v>
       </c>
       <c r="F219" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I219" s="137" t="s">
         <v>93</v>
@@ -11875,8 +11956,8 @@
       <c r="C221" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D221" s="217" t="s">
-        <v>316</v>
+      <c r="D221" s="216" t="s">
+        <v>313</v>
       </c>
       <c r="E221" s="18"/>
       <c r="F221" s="19"/>
@@ -11906,7 +11987,7 @@
         <v>90</v>
       </c>
       <c r="D223" s="22" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E223" s="18"/>
       <c r="F223" s="19"/>
@@ -12016,7 +12097,7 @@
       <c r="B231" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C231" s="208" t="s">
+      <c r="C231" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D231" s="48" t="s">
@@ -12036,19 +12117,19 @@
       </c>
     </row>
     <row r="232" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B232" s="220" t="s">
-        <v>349</v>
-      </c>
-      <c r="C232" s="221">
+      <c r="B232" s="219" t="s">
+        <v>346</v>
+      </c>
+      <c r="C232" s="220">
         <v>1</v>
       </c>
       <c r="D232" s="22" t="s">
-        <v>361</v>
-      </c>
-      <c r="E232" s="222">
+        <v>358</v>
+      </c>
+      <c r="E232" s="221">
         <v>43265</v>
       </c>
-      <c r="F232" s="223">
+      <c r="F232" s="222">
         <v>43265</v>
       </c>
       <c r="I232" s="137" t="s">
@@ -12059,19 +12140,19 @@
       </c>
     </row>
     <row r="233" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B233" s="220" t="s">
-        <v>349</v>
-      </c>
-      <c r="C233" s="221">
+      <c r="B233" s="219" t="s">
+        <v>346</v>
+      </c>
+      <c r="C233" s="220">
         <v>2</v>
       </c>
       <c r="D233" s="22" t="s">
-        <v>362</v>
-      </c>
-      <c r="E233" s="222">
+        <v>359</v>
+      </c>
+      <c r="E233" s="221">
         <v>43266</v>
       </c>
-      <c r="F233" s="223">
+      <c r="F233" s="222">
         <v>43266</v>
       </c>
       <c r="I233" s="137" t="s">
@@ -12134,17 +12215,17 @@
       <c r="B238" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C238" s="215" t="s">
-        <v>278</v>
+      <c r="C238" s="214" t="s">
+        <v>275</v>
       </c>
       <c r="D238" s="165" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E238" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F238" s="167" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="I238" s="137" t="s">
         <v>93</v>
@@ -12178,7 +12259,7 @@
         <v>135</v>
       </c>
       <c r="F240" s="112">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I240" s="137" t="s">
         <v>93</v>
@@ -12191,8 +12272,8 @@
       <c r="B241" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C241" s="209" t="s">
-        <v>347</v>
+      <c r="C241" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D241" s="15" t="s">
         <v>126</v>
@@ -12201,7 +12282,7 @@
         <v>56</v>
       </c>
       <c r="F241" s="133" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I241" s="137" t="s">
         <v>93</v>
@@ -12214,8 +12295,8 @@
       <c r="B242" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C242" s="210" t="s">
-        <v>336</v>
+      <c r="C242" s="209" t="s">
+        <v>333</v>
       </c>
       <c r="D242" s="18"/>
       <c r="E242" s="16" t="s">
@@ -12260,7 +12341,7 @@
         <v>50</v>
       </c>
       <c r="C244" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D244" s="15" t="s">
         <v>96</v>
@@ -12283,7 +12364,7 @@
         <v>57</v>
       </c>
       <c r="C245" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D245" s="15" t="s">
         <v>99</v>
@@ -12292,7 +12373,7 @@
         <v>62</v>
       </c>
       <c r="F245" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I245" s="137" t="s">
         <v>93</v>
@@ -12319,8 +12400,8 @@
       <c r="C247" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D247" s="217" t="s">
-        <v>317</v>
+      <c r="D247" s="216" t="s">
+        <v>314</v>
       </c>
       <c r="E247" s="18"/>
       <c r="F247" s="19"/>
@@ -12350,7 +12431,7 @@
         <v>90</v>
       </c>
       <c r="D249" s="22" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E249" s="18"/>
       <c r="F249" s="19"/>
@@ -12460,7 +12541,7 @@
       <c r="B257" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C257" s="208" t="s">
+      <c r="C257" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D257" s="48" t="s">
@@ -12480,19 +12561,19 @@
       </c>
     </row>
     <row r="258" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B258" s="220" t="s">
-        <v>348</v>
-      </c>
-      <c r="C258" s="221">
+      <c r="B258" s="219" t="s">
+        <v>345</v>
+      </c>
+      <c r="C258" s="220">
         <v>1</v>
       </c>
       <c r="D258" s="22" t="s">
-        <v>363</v>
-      </c>
-      <c r="E258" s="222">
+        <v>360</v>
+      </c>
+      <c r="E258" s="221">
         <v>43265</v>
       </c>
-      <c r="F258" s="223">
+      <c r="F258" s="222">
         <v>43265</v>
       </c>
       <c r="I258" s="137" t="s">
@@ -12568,17 +12649,17 @@
       <c r="B264" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C264" s="215" t="s">
-        <v>279</v>
+      <c r="C264" s="214" t="s">
+        <v>276</v>
       </c>
       <c r="D264" s="165" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E264" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F264" s="167" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I264" s="137" t="s">
         <v>93</v>
@@ -12612,7 +12693,7 @@
         <v>135</v>
       </c>
       <c r="F266" s="112">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I266" s="137" t="s">
         <v>93</v>
@@ -12625,8 +12706,8 @@
       <c r="B267" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C267" s="209" t="s">
-        <v>347</v>
+      <c r="C267" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D267" s="15" t="s">
         <v>126</v>
@@ -12635,7 +12716,7 @@
         <v>56</v>
       </c>
       <c r="F267" s="133" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I267" s="137" t="s">
         <v>93</v>
@@ -12648,8 +12729,8 @@
       <c r="B268" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C268" s="210" t="s">
-        <v>336</v>
+      <c r="C268" s="209" t="s">
+        <v>333</v>
       </c>
       <c r="D268" s="18"/>
       <c r="E268" s="16" t="s">
@@ -12694,7 +12775,7 @@
         <v>50</v>
       </c>
       <c r="C270" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D270" s="15" t="s">
         <v>96</v>
@@ -12717,7 +12798,7 @@
         <v>57</v>
       </c>
       <c r="C271" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D271" s="15" t="s">
         <v>99</v>
@@ -12726,7 +12807,7 @@
         <v>62</v>
       </c>
       <c r="F271" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I271" s="137" t="s">
         <v>93</v>
@@ -12753,8 +12834,8 @@
       <c r="C273" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D273" s="217" t="s">
-        <v>313</v>
+      <c r="D273" s="216" t="s">
+        <v>310</v>
       </c>
       <c r="E273" s="18"/>
       <c r="F273" s="19"/>
@@ -12784,7 +12865,7 @@
         <v>90</v>
       </c>
       <c r="D275" s="22" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E275" s="18"/>
       <c r="F275" s="19"/>
@@ -12894,7 +12975,7 @@
       <c r="B283" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C283" s="208" t="s">
+      <c r="C283" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D283" s="48" t="s">
@@ -12914,14 +12995,14 @@
       </c>
     </row>
     <row r="284" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B284" s="220" t="s">
-        <v>348</v>
-      </c>
-      <c r="C284" s="221">
+      <c r="B284" s="219" t="s">
+        <v>345</v>
+      </c>
+      <c r="C284" s="220">
         <v>1</v>
       </c>
       <c r="D284" s="22" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E284" s="27">
         <v>43265</v>
@@ -12937,14 +13018,14 @@
       </c>
     </row>
     <row r="285" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B285" s="220" t="s">
-        <v>347</v>
-      </c>
-      <c r="C285" s="221">
+      <c r="B285" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C285" s="220">
         <v>2</v>
       </c>
       <c r="D285" s="22" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="E285" s="27">
         <v>43266</v>
@@ -13012,17 +13093,17 @@
       <c r="B290" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C290" s="215" t="s">
-        <v>280</v>
+      <c r="C290" s="214" t="s">
+        <v>277</v>
       </c>
       <c r="D290" s="165" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E290" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F290" s="167" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I290" s="137" t="s">
         <v>93</v>
@@ -13069,8 +13150,8 @@
       <c r="B293" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C293" s="209" t="s">
-        <v>347</v>
+      <c r="C293" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D293" s="15" t="s">
         <v>126</v>
@@ -13079,7 +13160,7 @@
         <v>56</v>
       </c>
       <c r="F293" s="133" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I293" s="137" t="s">
         <v>93</v>
@@ -13092,8 +13173,8 @@
       <c r="B294" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C294" s="210" t="s">
-        <v>336</v>
+      <c r="C294" s="209" t="s">
+        <v>333</v>
       </c>
       <c r="D294" s="18"/>
       <c r="E294" s="16" t="s">
@@ -13114,7 +13195,7 @@
         <v>44</v>
       </c>
       <c r="C295" s="132" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D295" s="49" t="str">
         <f>IF(C295="","WARNING - Please enter a Probability.","")</f>
@@ -13138,7 +13219,7 @@
         <v>50</v>
       </c>
       <c r="C296" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D296" s="15" t="s">
         <v>96</v>
@@ -13170,7 +13251,7 @@
         <v>62</v>
       </c>
       <c r="F297" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I297" s="137" t="s">
         <v>93</v>
@@ -13197,8 +13278,8 @@
       <c r="C299" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D299" s="217" t="s">
-        <v>314</v>
+      <c r="D299" s="216" t="s">
+        <v>311</v>
       </c>
       <c r="E299" s="18"/>
       <c r="F299" s="19"/>
@@ -13228,7 +13309,7 @@
         <v>90</v>
       </c>
       <c r="D301" s="22" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E301" s="18"/>
       <c r="F301" s="19"/>
@@ -13338,7 +13419,7 @@
       <c r="B309" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C309" s="208" t="s">
+      <c r="C309" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D309" s="48" t="s">
@@ -13358,19 +13439,19 @@
       </c>
     </row>
     <row r="310" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B310" s="220" t="s">
-        <v>348</v>
-      </c>
-      <c r="C310" s="221">
+      <c r="B310" s="219" t="s">
+        <v>345</v>
+      </c>
+      <c r="C310" s="220">
         <v>1</v>
       </c>
       <c r="D310" s="22" t="s">
-        <v>367</v>
-      </c>
-      <c r="E310" s="222">
+        <v>364</v>
+      </c>
+      <c r="E310" s="221">
         <v>43265</v>
       </c>
-      <c r="F310" s="223">
+      <c r="F310" s="222">
         <v>43265</v>
       </c>
       <c r="I310" s="137" t="s">
@@ -13381,19 +13462,19 @@
       </c>
     </row>
     <row r="311" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B311" s="220" t="s">
-        <v>348</v>
-      </c>
-      <c r="C311" s="221">
+      <c r="B311" s="219" t="s">
+        <v>345</v>
+      </c>
+      <c r="C311" s="220">
         <v>2</v>
       </c>
       <c r="D311" s="22" t="s">
-        <v>368</v>
-      </c>
-      <c r="E311" s="222">
+        <v>365</v>
+      </c>
+      <c r="E311" s="221">
         <v>43266</v>
       </c>
-      <c r="F311" s="223">
+      <c r="F311" s="222">
         <v>43266</v>
       </c>
       <c r="I311" s="137" t="s">
@@ -13459,17 +13540,17 @@
       <c r="B316" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C316" s="215" t="s">
-        <v>281</v>
+      <c r="C316" s="214" t="s">
+        <v>278</v>
       </c>
       <c r="D316" s="165" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E316" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F316" s="167" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I316" s="137" t="s">
         <v>93</v>
@@ -13503,7 +13584,7 @@
         <v>135</v>
       </c>
       <c r="F318" s="112">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I318" s="137" t="s">
         <v>93</v>
@@ -13516,8 +13597,8 @@
       <c r="B319" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C319" s="209" t="s">
-        <v>347</v>
+      <c r="C319" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D319" s="15" t="s">
         <v>126</v>
@@ -13526,7 +13607,7 @@
         <v>56</v>
       </c>
       <c r="F319" s="133" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I319" s="137" t="s">
         <v>93</v>
@@ -13539,8 +13620,8 @@
       <c r="B320" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C320" s="209" t="s">
-        <v>336</v>
+      <c r="C320" s="208" t="s">
+        <v>333</v>
       </c>
       <c r="D320" s="18"/>
       <c r="E320" s="16" t="s">
@@ -13585,7 +13666,7 @@
         <v>50</v>
       </c>
       <c r="C322" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D322" s="15" t="s">
         <v>96</v>
@@ -13608,7 +13689,7 @@
         <v>57</v>
       </c>
       <c r="C323" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D323" s="15" t="s">
         <v>99</v>
@@ -13617,7 +13698,7 @@
         <v>62</v>
       </c>
       <c r="F323" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I323" s="137" t="s">
         <v>93</v>
@@ -13644,8 +13725,8 @@
       <c r="C325" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D325" s="217" t="s">
-        <v>318</v>
+      <c r="D325" s="216" t="s">
+        <v>315</v>
       </c>
       <c r="E325" s="18"/>
       <c r="F325" s="19"/>
@@ -13675,7 +13756,7 @@
         <v>90</v>
       </c>
       <c r="D327" s="22" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E327" s="18"/>
       <c r="F327" s="19"/>
@@ -13785,7 +13866,7 @@
       <c r="B335" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C335" s="208" t="s">
+      <c r="C335" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D335" s="48" t="s">
@@ -13805,19 +13886,19 @@
       </c>
     </row>
     <row r="336" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B336" s="220" t="s">
-        <v>348</v>
-      </c>
-      <c r="C336" s="221">
+      <c r="B336" s="219" t="s">
+        <v>345</v>
+      </c>
+      <c r="C336" s="220">
         <v>1</v>
       </c>
       <c r="D336" s="22" t="s">
-        <v>384</v>
-      </c>
-      <c r="E336" s="222">
+        <v>381</v>
+      </c>
+      <c r="E336" s="221">
         <v>43265</v>
       </c>
-      <c r="F336" s="223">
+      <c r="F336" s="222">
         <v>43265</v>
       </c>
       <c r="I336" s="137" t="s">
@@ -13896,17 +13977,17 @@
       <c r="B342" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C342" s="215" t="s">
-        <v>282</v>
+      <c r="C342" s="214" t="s">
+        <v>279</v>
       </c>
       <c r="D342" s="165" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E342" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F342" s="167" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I342" s="137" t="s">
         <v>93</v>
@@ -13953,8 +14034,8 @@
       <c r="B345" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C345" s="209" t="s">
-        <v>347</v>
+      <c r="C345" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D345" s="15" t="s">
         <v>126</v>
@@ -13976,8 +14057,8 @@
       <c r="B346" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C346" s="209" t="s">
-        <v>336</v>
+      <c r="C346" s="208" t="s">
+        <v>333</v>
       </c>
       <c r="D346" s="18"/>
       <c r="E346" s="16" t="s">
@@ -13998,7 +14079,7 @@
         <v>44</v>
       </c>
       <c r="C347" s="132" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D347" s="49" t="str">
         <f>IF(C347="","WARNING - Please enter a Probability.","")</f>
@@ -14022,7 +14103,7 @@
         <v>50</v>
       </c>
       <c r="C348" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D348" s="15" t="s">
         <v>96</v>
@@ -14045,7 +14126,7 @@
         <v>57</v>
       </c>
       <c r="C349" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D349" s="15" t="s">
         <v>99</v>
@@ -14054,7 +14135,7 @@
         <v>62</v>
       </c>
       <c r="F349" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I349" s="137" t="s">
         <v>93</v>
@@ -14081,8 +14162,8 @@
       <c r="C351" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D351" s="217" t="s">
-        <v>320</v>
+      <c r="D351" s="216" t="s">
+        <v>317</v>
       </c>
       <c r="E351" s="18"/>
       <c r="F351" s="19"/>
@@ -14112,7 +14193,7 @@
         <v>90</v>
       </c>
       <c r="D353" s="22" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E353" s="18"/>
       <c r="F353" s="19"/>
@@ -14222,7 +14303,7 @@
       <c r="B361" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C361" s="208" t="s">
+      <c r="C361" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D361" s="48" t="s">
@@ -14242,19 +14323,19 @@
       </c>
     </row>
     <row r="362" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B362" s="220" t="s">
-        <v>336</v>
-      </c>
-      <c r="C362" s="221">
+      <c r="B362" s="219" t="s">
+        <v>333</v>
+      </c>
+      <c r="C362" s="220">
         <v>1</v>
       </c>
       <c r="D362" s="22" t="s">
-        <v>369</v>
-      </c>
-      <c r="E362" s="222">
+        <v>366</v>
+      </c>
+      <c r="E362" s="221">
         <v>43265</v>
       </c>
-      <c r="F362" s="223">
+      <c r="F362" s="222">
         <v>43265</v>
       </c>
       <c r="I362" s="137" t="s">
@@ -14333,17 +14414,17 @@
       <c r="B368" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C368" s="215" t="s">
-        <v>283</v>
+      <c r="C368" s="214" t="s">
+        <v>280</v>
       </c>
       <c r="D368" s="165" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E368" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F368" s="167" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="I368" s="137" t="s">
         <v>93</v>
@@ -14377,7 +14458,7 @@
         <v>135</v>
       </c>
       <c r="F370" s="112">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I370" s="137" t="s">
         <v>93</v>
@@ -14390,8 +14471,8 @@
       <c r="B371" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C371" s="209" t="s">
-        <v>347</v>
+      <c r="C371" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D371" s="15" t="s">
         <v>126</v>
@@ -14413,8 +14494,8 @@
       <c r="B372" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C372" s="209" t="s">
-        <v>336</v>
+      <c r="C372" s="208" t="s">
+        <v>333</v>
       </c>
       <c r="D372" s="18"/>
       <c r="E372" s="16" t="s">
@@ -14459,7 +14540,7 @@
         <v>50</v>
       </c>
       <c r="C374" s="132" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D374" s="15" t="s">
         <v>96</v>
@@ -14482,7 +14563,7 @@
         <v>57</v>
       </c>
       <c r="C375" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D375" s="15" t="s">
         <v>99</v>
@@ -14491,7 +14572,7 @@
         <v>62</v>
       </c>
       <c r="F375" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I375" s="137" t="s">
         <v>93</v>
@@ -14518,8 +14599,8 @@
       <c r="C377" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D377" s="217" t="s">
-        <v>322</v>
+      <c r="D377" s="216" t="s">
+        <v>319</v>
       </c>
       <c r="E377" s="18"/>
       <c r="F377" s="19"/>
@@ -14549,7 +14630,7 @@
         <v>90</v>
       </c>
       <c r="D379" s="22" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E379" s="18"/>
       <c r="F379" s="19"/>
@@ -14659,7 +14740,7 @@
       <c r="B387" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C387" s="208" t="s">
+      <c r="C387" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D387" s="48" t="s">
@@ -14680,13 +14761,13 @@
     </row>
     <row r="388" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B388" s="25" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C388" s="26">
         <v>1</v>
       </c>
       <c r="D388" s="22" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E388" s="27">
         <v>43265</v>
@@ -14767,17 +14848,17 @@
       <c r="B394" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C394" s="215" t="s">
-        <v>284</v>
+      <c r="C394" s="214" t="s">
+        <v>281</v>
       </c>
       <c r="D394" s="165" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E394" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F394" s="167" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I394" s="137" t="s">
         <v>93</v>
@@ -14811,7 +14892,7 @@
         <v>135</v>
       </c>
       <c r="F396" s="112">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I396" s="137" t="s">
         <v>93</v>
@@ -14824,8 +14905,8 @@
       <c r="B397" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C397" s="209" t="s">
-        <v>347</v>
+      <c r="C397" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D397" s="15" t="s">
         <v>126</v>
@@ -14834,7 +14915,7 @@
         <v>56</v>
       </c>
       <c r="F397" s="133" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I397" s="137" t="s">
         <v>93</v>
@@ -14847,8 +14928,8 @@
       <c r="B398" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C398" s="209" t="s">
-        <v>349</v>
+      <c r="C398" s="208" t="s">
+        <v>346</v>
       </c>
       <c r="D398" s="18"/>
       <c r="E398" s="16" t="s">
@@ -14893,7 +14974,7 @@
         <v>50</v>
       </c>
       <c r="C400" s="132" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D400" s="15" t="s">
         <v>96</v>
@@ -14916,7 +14997,7 @@
         <v>57</v>
       </c>
       <c r="C401" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D401" s="15" t="s">
         <v>99</v>
@@ -14925,7 +15006,7 @@
         <v>62</v>
       </c>
       <c r="F401" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I401" s="137" t="s">
         <v>93</v>
@@ -14952,8 +15033,8 @@
       <c r="C403" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D403" s="217" t="s">
-        <v>325</v>
+      <c r="D403" s="216" t="s">
+        <v>322</v>
       </c>
       <c r="E403" s="18"/>
       <c r="F403" s="19"/>
@@ -14983,7 +15064,7 @@
         <v>90</v>
       </c>
       <c r="D405" s="22" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E405" s="18"/>
       <c r="F405" s="19"/>
@@ -15093,7 +15174,7 @@
       <c r="B413" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C413" s="208" t="s">
+      <c r="C413" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D413" s="48" t="s">
@@ -15114,13 +15195,13 @@
     </row>
     <row r="414" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B414" s="25" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C414" s="26">
         <v>1</v>
       </c>
       <c r="D414" s="22" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E414" s="27">
         <v>43265</v>
@@ -15137,13 +15218,13 @@
     </row>
     <row r="415" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B415" s="25" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C415" s="26">
         <v>2</v>
       </c>
       <c r="D415" s="22" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E415" s="27">
         <v>43266</v>
@@ -15211,17 +15292,17 @@
       <c r="B420" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C420" s="215" t="s">
-        <v>285</v>
+      <c r="C420" s="214" t="s">
+        <v>282</v>
       </c>
       <c r="D420" s="165" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E420" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F420" s="167" t="s">
-        <v>104</v>
+        <v>378</v>
       </c>
       <c r="I420" s="137" t="s">
         <v>93</v>
@@ -15255,7 +15336,7 @@
         <v>135</v>
       </c>
       <c r="F422" s="112">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I422" s="137" t="s">
         <v>93</v>
@@ -15268,8 +15349,8 @@
       <c r="B423" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C423" s="209" t="s">
-        <v>347</v>
+      <c r="C423" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D423" s="15" t="s">
         <v>126</v>
@@ -15291,8 +15372,8 @@
       <c r="B424" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C424" s="209" t="s">
-        <v>336</v>
+      <c r="C424" s="208" t="s">
+        <v>333</v>
       </c>
       <c r="D424" s="18"/>
       <c r="E424" s="16" t="s">
@@ -15313,7 +15394,7 @@
         <v>44</v>
       </c>
       <c r="C425" s="132" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D425" s="49" t="str">
         <f>IF(C425="","WARNING - Please enter a Probability.","")</f>
@@ -15360,7 +15441,7 @@
         <v>57</v>
       </c>
       <c r="C427" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D427" s="15" t="s">
         <v>99</v>
@@ -15369,7 +15450,7 @@
         <v>62</v>
       </c>
       <c r="F427" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I427" s="137" t="s">
         <v>93</v>
@@ -15396,8 +15477,8 @@
       <c r="C429" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D429" s="217" t="s">
-        <v>327</v>
+      <c r="D429" s="216" t="s">
+        <v>324</v>
       </c>
       <c r="E429" s="18"/>
       <c r="F429" s="19"/>
@@ -15427,7 +15508,7 @@
         <v>90</v>
       </c>
       <c r="D431" s="22" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E431" s="18"/>
       <c r="F431" s="19"/>
@@ -15537,7 +15618,7 @@
       <c r="B439" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C439" s="208" t="s">
+      <c r="C439" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D439" s="48" t="s">
@@ -15557,19 +15638,19 @@
       </c>
     </row>
     <row r="440" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B440" s="220" t="s">
-        <v>349</v>
-      </c>
-      <c r="C440" s="221">
+      <c r="B440" s="219" t="s">
+        <v>346</v>
+      </c>
+      <c r="C440" s="220">
         <v>1</v>
       </c>
       <c r="D440" s="22" t="s">
-        <v>373</v>
-      </c>
-      <c r="E440" s="222">
+        <v>370</v>
+      </c>
+      <c r="E440" s="221">
         <v>43265</v>
       </c>
-      <c r="F440" s="223">
+      <c r="F440" s="222">
         <v>43265</v>
       </c>
       <c r="I440" s="137" t="s">
@@ -15580,19 +15661,19 @@
       </c>
     </row>
     <row r="441" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B441" s="220" t="s">
-        <v>349</v>
-      </c>
-      <c r="C441" s="221">
+      <c r="B441" s="219" t="s">
+        <v>346</v>
+      </c>
+      <c r="C441" s="220">
         <v>2</v>
       </c>
       <c r="D441" s="22" t="s">
-        <v>375</v>
-      </c>
-      <c r="E441" s="222">
+        <v>372</v>
+      </c>
+      <c r="E441" s="221">
         <v>43266</v>
       </c>
-      <c r="F441" s="223">
+      <c r="F441" s="222">
         <v>43266</v>
       </c>
       <c r="I441" s="137" t="s">
@@ -15655,17 +15736,17 @@
       <c r="B446" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C446" s="215" t="s">
-        <v>286</v>
+      <c r="C446" s="214" t="s">
+        <v>283</v>
       </c>
       <c r="D446" s="165" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E446" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F446" s="167" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I446" s="137" t="s">
         <v>93</v>
@@ -15699,7 +15780,7 @@
         <v>135</v>
       </c>
       <c r="F448" s="112">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I448" s="137" t="s">
         <v>93</v>
@@ -15712,8 +15793,8 @@
       <c r="B449" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C449" s="209" t="s">
-        <v>347</v>
+      <c r="C449" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D449" s="15" t="s">
         <v>126</v>
@@ -15735,8 +15816,8 @@
       <c r="B450" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C450" s="209" t="s">
-        <v>336</v>
+      <c r="C450" s="208" t="s">
+        <v>333</v>
       </c>
       <c r="D450" s="18"/>
       <c r="E450" s="16" t="s">
@@ -15804,7 +15885,7 @@
         <v>57</v>
       </c>
       <c r="C453" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D453" s="15" t="s">
         <v>99</v>
@@ -15813,7 +15894,7 @@
         <v>62</v>
       </c>
       <c r="F453" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I453" s="137" t="s">
         <v>93</v>
@@ -15840,8 +15921,8 @@
       <c r="C455" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D455" s="217" t="s">
-        <v>328</v>
+      <c r="D455" s="216" t="s">
+        <v>325</v>
       </c>
       <c r="E455" s="18"/>
       <c r="F455" s="19"/>
@@ -15871,7 +15952,7 @@
         <v>90</v>
       </c>
       <c r="D457" s="22" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E457" s="18"/>
       <c r="F457" s="19"/>
@@ -15981,7 +16062,7 @@
       <c r="B465" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C465" s="208" t="s">
+      <c r="C465" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D465" s="48" t="s">
@@ -16001,19 +16082,19 @@
       </c>
     </row>
     <row r="466" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B466" s="220" t="s">
-        <v>336</v>
-      </c>
-      <c r="C466" s="221">
+      <c r="B466" s="219" t="s">
+        <v>333</v>
+      </c>
+      <c r="C466" s="220">
         <v>1</v>
       </c>
       <c r="D466" s="22" t="s">
-        <v>376</v>
-      </c>
-      <c r="E466" s="222">
+        <v>373</v>
+      </c>
+      <c r="E466" s="221">
         <v>43265</v>
       </c>
-      <c r="F466" s="223">
+      <c r="F466" s="222">
         <v>43265</v>
       </c>
       <c r="I466" s="137" t="s">
@@ -16089,17 +16170,17 @@
       <c r="B472" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C472" s="215" t="s">
-        <v>287</v>
+      <c r="C472" s="214" t="s">
+        <v>284</v>
       </c>
       <c r="D472" s="165" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E472" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F472" s="167" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I472" s="137" t="s">
         <v>93</v>
@@ -16133,7 +16214,7 @@
         <v>135</v>
       </c>
       <c r="F474" s="112">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I474" s="137" t="s">
         <v>93</v>
@@ -16146,8 +16227,8 @@
       <c r="B475" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C475" s="209" t="s">
-        <v>347</v>
+      <c r="C475" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D475" s="15" t="s">
         <v>126</v>
@@ -16169,8 +16250,8 @@
       <c r="B476" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C476" s="209" t="s">
-        <v>336</v>
+      <c r="C476" s="208" t="s">
+        <v>333</v>
       </c>
       <c r="D476" s="18"/>
       <c r="E476" s="16" t="s">
@@ -16215,7 +16296,7 @@
         <v>50</v>
       </c>
       <c r="C478" s="132" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D478" s="15" t="s">
         <v>96</v>
@@ -16238,7 +16319,7 @@
         <v>57</v>
       </c>
       <c r="C479" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D479" s="15" t="s">
         <v>99</v>
@@ -16247,7 +16328,7 @@
         <v>62</v>
       </c>
       <c r="F479" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I479" s="137" t="s">
         <v>93</v>
@@ -16274,8 +16355,8 @@
       <c r="C481" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D481" s="218" t="s">
-        <v>342</v>
+      <c r="D481" s="217" t="s">
+        <v>339</v>
       </c>
       <c r="E481" s="18"/>
       <c r="F481" s="19"/>
@@ -16305,7 +16386,7 @@
         <v>90</v>
       </c>
       <c r="D483" s="22" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E483" s="18"/>
       <c r="F483" s="19"/>
@@ -16415,7 +16496,7 @@
       <c r="B491" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C491" s="208" t="s">
+      <c r="C491" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D491" s="48" t="s">
@@ -16435,19 +16516,19 @@
       </c>
     </row>
     <row r="492" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B492" s="220" t="s">
-        <v>348</v>
-      </c>
-      <c r="C492" s="221">
+      <c r="B492" s="219" t="s">
+        <v>345</v>
+      </c>
+      <c r="C492" s="220">
         <v>1</v>
       </c>
       <c r="D492" s="172" t="s">
-        <v>346</v>
-      </c>
-      <c r="E492" s="222">
+        <v>343</v>
+      </c>
+      <c r="E492" s="221">
         <v>43265</v>
       </c>
-      <c r="F492" s="223">
+      <c r="F492" s="222">
         <v>43265</v>
       </c>
       <c r="I492" s="137" t="s">
@@ -16458,19 +16539,19 @@
       </c>
     </row>
     <row r="493" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B493" s="220" t="s">
-        <v>348</v>
-      </c>
-      <c r="C493" s="221">
+      <c r="B493" s="219" t="s">
+        <v>345</v>
+      </c>
+      <c r="C493" s="220">
         <v>2</v>
       </c>
       <c r="D493" s="172" t="s">
-        <v>345</v>
-      </c>
-      <c r="E493" s="222">
+        <v>342</v>
+      </c>
+      <c r="E493" s="221">
         <v>43266</v>
       </c>
-      <c r="F493" s="223">
+      <c r="F493" s="222">
         <v>43266</v>
       </c>
       <c r="I493" s="137" t="s">
@@ -16481,19 +16562,19 @@
       </c>
     </row>
     <row r="494" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B494" s="220" t="s">
-        <v>348</v>
-      </c>
-      <c r="C494" s="221">
+      <c r="B494" s="219" t="s">
+        <v>345</v>
+      </c>
+      <c r="C494" s="220">
         <v>3</v>
       </c>
       <c r="D494" s="172" t="s">
-        <v>344</v>
-      </c>
-      <c r="E494" s="222">
+        <v>341</v>
+      </c>
+      <c r="E494" s="221">
         <v>43267</v>
       </c>
-      <c r="F494" s="223">
+      <c r="F494" s="222">
         <v>43267</v>
       </c>
       <c r="I494" s="137" t="s">
@@ -16543,17 +16624,17 @@
       <c r="B498" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C498" s="215" t="s">
-        <v>289</v>
+      <c r="C498" s="214" t="s">
+        <v>286</v>
       </c>
       <c r="D498" s="165" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E498" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F498" s="167" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I498" s="137" t="s">
         <v>93</v>
@@ -16566,7 +16647,7 @@
       <c r="B499" s="189" t="s">
         <v>215</v>
       </c>
-      <c r="C499" s="214"/>
+      <c r="C499" s="213"/>
       <c r="D499" s="191"/>
       <c r="E499" s="21"/>
       <c r="F499" s="192"/>
@@ -16587,7 +16668,7 @@
         <v>135</v>
       </c>
       <c r="F500" s="112">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I500" s="137" t="s">
         <v>93</v>
@@ -16600,8 +16681,8 @@
       <c r="B501" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C501" s="209" t="s">
-        <v>347</v>
+      <c r="C501" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D501" s="15" t="s">
         <v>126</v>
@@ -16623,8 +16704,8 @@
       <c r="B502" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C502" s="209" t="s">
-        <v>336</v>
+      <c r="C502" s="208" t="s">
+        <v>333</v>
       </c>
       <c r="D502" s="18"/>
       <c r="E502" s="16" t="s">
@@ -16645,7 +16726,7 @@
         <v>44</v>
       </c>
       <c r="C503" s="132" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D503" s="49" t="str">
         <f>IF(C503="","WARNING - Please enter a Probability.","")</f>
@@ -16669,7 +16750,7 @@
         <v>50</v>
       </c>
       <c r="C504" s="132" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D504" s="15" t="s">
         <v>96</v>
@@ -16692,7 +16773,7 @@
         <v>57</v>
       </c>
       <c r="C505" s="132" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D505" s="15" t="s">
         <v>99</v>
@@ -16701,7 +16782,7 @@
         <v>62</v>
       </c>
       <c r="F505" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I505" s="137" t="s">
         <v>93</v>
@@ -16728,8 +16809,8 @@
       <c r="C507" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D507" s="217" t="s">
-        <v>331</v>
+      <c r="D507" s="216" t="s">
+        <v>328</v>
       </c>
       <c r="E507" s="18"/>
       <c r="F507" s="19"/>
@@ -16759,7 +16840,7 @@
         <v>90</v>
       </c>
       <c r="D509" s="22" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E509" s="18"/>
       <c r="F509" s="19"/>
@@ -16869,7 +16950,7 @@
       <c r="B517" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C517" s="208" t="s">
+      <c r="C517" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D517" s="48" t="s">
@@ -16889,19 +16970,19 @@
       </c>
     </row>
     <row r="518" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B518" s="220" t="s">
-        <v>348</v>
-      </c>
-      <c r="C518" s="221">
+      <c r="B518" s="219" t="s">
+        <v>345</v>
+      </c>
+      <c r="C518" s="220">
         <v>1</v>
       </c>
       <c r="D518" s="172" t="s">
-        <v>343</v>
-      </c>
-      <c r="E518" s="222">
+        <v>340</v>
+      </c>
+      <c r="E518" s="221">
         <v>43265</v>
       </c>
-      <c r="F518" s="223">
+      <c r="F518" s="222">
         <v>43265</v>
       </c>
       <c r="I518" s="137" t="s">
@@ -16912,19 +16993,19 @@
       </c>
     </row>
     <row r="519" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B519" s="220" t="s">
-        <v>348</v>
-      </c>
-      <c r="C519" s="221">
+      <c r="B519" s="219" t="s">
+        <v>345</v>
+      </c>
+      <c r="C519" s="220">
         <v>2</v>
       </c>
       <c r="D519" s="172" t="s">
-        <v>344</v>
-      </c>
-      <c r="E519" s="222">
+        <v>341</v>
+      </c>
+      <c r="E519" s="221">
         <v>43266</v>
       </c>
-      <c r="F519" s="223">
+      <c r="F519" s="222">
         <v>43266</v>
       </c>
       <c r="I519" s="137" t="s">
@@ -16987,17 +17068,17 @@
       <c r="B524" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C524" s="215" t="s">
-        <v>290</v>
+      <c r="C524" s="214" t="s">
+        <v>287</v>
       </c>
       <c r="D524" s="165" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E524" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F524" s="167" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I524" s="137" t="s">
         <v>93</v>
@@ -17010,7 +17091,7 @@
       <c r="B525" s="189" t="s">
         <v>215</v>
       </c>
-      <c r="C525" s="214"/>
+      <c r="C525" s="213"/>
       <c r="D525" s="191"/>
       <c r="E525" s="21"/>
       <c r="F525" s="192"/>
@@ -17031,7 +17112,7 @@
         <v>135</v>
       </c>
       <c r="F526" s="112">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I526" s="137" t="s">
         <v>93</v>
@@ -17044,8 +17125,8 @@
       <c r="B527" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C527" s="209" t="s">
-        <v>347</v>
+      <c r="C527" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D527" s="15" t="s">
         <v>126</v>
@@ -17054,7 +17135,7 @@
         <v>56</v>
       </c>
       <c r="F527" s="133" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="I527" s="137" t="s">
         <v>93</v>
@@ -17067,8 +17148,8 @@
       <c r="B528" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C528" s="209" t="s">
-        <v>336</v>
+      <c r="C528" s="208" t="s">
+        <v>333</v>
       </c>
       <c r="D528" s="18"/>
       <c r="E528" s="16" t="s">
@@ -17089,7 +17170,7 @@
         <v>44</v>
       </c>
       <c r="C529" s="132" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D529" s="49" t="str">
         <f>IF(C529="","WARNING - Please enter a Probability.","")</f>
@@ -17145,7 +17226,7 @@
         <v>62</v>
       </c>
       <c r="F531" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I531" s="137" t="s">
         <v>93</v>
@@ -17172,8 +17253,8 @@
       <c r="C533" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D533" s="217" t="s">
-        <v>333</v>
+      <c r="D533" s="216" t="s">
+        <v>330</v>
       </c>
       <c r="E533" s="18"/>
       <c r="F533" s="19"/>
@@ -17203,7 +17284,7 @@
         <v>90</v>
       </c>
       <c r="D535" s="22" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E535" s="18"/>
       <c r="F535" s="19"/>
@@ -17255,12 +17336,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="539" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="539" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B539" s="20"/>
       <c r="C539" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="D539" s="22"/>
+      <c r="D539" s="22" t="s">
+        <v>382</v>
+      </c>
       <c r="E539" s="18"/>
       <c r="F539" s="19"/>
       <c r="I539" s="137" t="s">
@@ -17313,7 +17396,7 @@
       <c r="B543" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C543" s="208" t="s">
+      <c r="C543" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D543" s="48" t="s">
@@ -17333,19 +17416,19 @@
       </c>
     </row>
     <row r="544" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B544" s="220" t="s">
-        <v>347</v>
-      </c>
-      <c r="C544" s="221">
+      <c r="B544" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C544" s="220">
         <v>1</v>
       </c>
       <c r="D544" s="22" t="s">
-        <v>377</v>
-      </c>
-      <c r="E544" s="222">
+        <v>374</v>
+      </c>
+      <c r="E544" s="221">
         <v>43265</v>
       </c>
-      <c r="F544" s="223">
+      <c r="F544" s="222">
         <v>43265</v>
       </c>
       <c r="I544" s="137" t="s">
@@ -17421,17 +17504,17 @@
       <c r="B550" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C550" s="215" t="s">
-        <v>291</v>
+      <c r="C550" s="214" t="s">
+        <v>288</v>
       </c>
       <c r="D550" s="165" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E550" s="166" t="s">
         <v>51</v>
       </c>
       <c r="F550" s="167" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="I550" s="137" t="s">
         <v>93</v>
@@ -17444,7 +17527,7 @@
       <c r="B551" s="189" t="s">
         <v>215</v>
       </c>
-      <c r="C551" s="214"/>
+      <c r="C551" s="213"/>
       <c r="D551" s="191"/>
       <c r="E551" s="21"/>
       <c r="F551" s="192"/>
@@ -17465,7 +17548,7 @@
         <v>135</v>
       </c>
       <c r="F552" s="112">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I552" s="137" t="s">
         <v>93</v>
@@ -17478,8 +17561,8 @@
       <c r="B553" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C553" s="209" t="s">
-        <v>347</v>
+      <c r="C553" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D553" s="15" t="s">
         <v>126</v>
@@ -17488,7 +17571,7 @@
         <v>56</v>
       </c>
       <c r="F553" s="133" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="I553" s="137" t="s">
         <v>93</v>
@@ -17501,8 +17584,8 @@
       <c r="B554" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C554" s="209" t="s">
-        <v>347</v>
+      <c r="C554" s="208" t="s">
+        <v>344</v>
       </c>
       <c r="D554" s="18"/>
       <c r="E554" s="16" t="s">
@@ -17523,7 +17606,7 @@
         <v>44</v>
       </c>
       <c r="C555" s="132" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D555" s="49" t="str">
         <f>IF(C555="","WARNING - Please enter a Probability.","")</f>
@@ -17579,7 +17662,7 @@
         <v>62</v>
       </c>
       <c r="F557" s="174">
-        <v>43265</v>
+        <v>43279</v>
       </c>
       <c r="I557" s="137" t="s">
         <v>93</v>
@@ -17606,8 +17689,8 @@
       <c r="C559" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D559" s="217" t="s">
-        <v>335</v>
+      <c r="D559" s="216" t="s">
+        <v>332</v>
       </c>
       <c r="E559" s="18"/>
       <c r="F559" s="19"/>
@@ -17637,7 +17720,7 @@
         <v>90</v>
       </c>
       <c r="D561" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E561" s="18"/>
       <c r="F561" s="19"/>
@@ -17689,12 +17772,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="565" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="565" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B565" s="20"/>
       <c r="C565" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="D565" s="22"/>
+      <c r="D565" s="22" t="s">
+        <v>382</v>
+      </c>
       <c r="E565" s="18"/>
       <c r="F565" s="19"/>
       <c r="I565" s="137" t="s">
@@ -17747,7 +17832,7 @@
       <c r="B569" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C569" s="208" t="s">
+      <c r="C569" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D569" s="48" t="s">
@@ -17767,19 +17852,19 @@
       </c>
     </row>
     <row r="570" spans="2:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B570" s="220" t="s">
-        <v>347</v>
-      </c>
-      <c r="C570" s="221">
+      <c r="B570" s="219" t="s">
+        <v>344</v>
+      </c>
+      <c r="C570" s="220">
         <v>1</v>
       </c>
       <c r="D570" s="22" t="s">
-        <v>360</v>
-      </c>
-      <c r="E570" s="222">
+        <v>357</v>
+      </c>
+      <c r="E570" s="221">
         <v>43265</v>
       </c>
-      <c r="F570" s="223">
+      <c r="F570" s="222">
         <v>43265</v>
       </c>
       <c r="I570" s="137" t="s">
@@ -18181,7 +18266,7 @@
       <c r="B595" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C595" s="208" t="s">
+      <c r="C595" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D595" s="48" t="s">
@@ -18645,7 +18730,7 @@
       <c r="B621" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C621" s="208" t="s">
+      <c r="C621" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D621" s="48" t="s">
@@ -19109,7 +19194,7 @@
       <c r="B647" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C647" s="208" t="s">
+      <c r="C647" s="207" t="s">
         <v>174</v>
       </c>
       <c r="D647" s="48" t="s">
@@ -21812,11 +21897,11 @@
       </c>
       <c r="I7" s="123">
         <f>Exposure!E7</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J7" s="94">
         <f>Exposure!F7</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -21868,11 +21953,11 @@
       </c>
       <c r="I9" s="124">
         <f>SUM(I6:I8)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J9" s="95">
         <f>SUM(J6:J8)</f>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -21926,7 +22011,7 @@
       </c>
       <c r="B12" s="157">
         <f>IF($A12="","",'Detalle del Riesgo'!F5)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C12" s="158" t="str">
         <f>IF($A12="","",LEFT('Detalle del Riesgo'!D10,1))</f>
@@ -21968,7 +22053,7 @@
       </c>
       <c r="B13" s="157">
         <f>IF($A13="","",'Detalle del Riesgo'!F32)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C13" s="158" t="str">
         <f>IF($A13="","",LEFT('Detalle del Riesgo'!D37,1))</f>
@@ -22010,7 +22095,7 @@
       </c>
       <c r="B14" s="157">
         <f>IF($A14="","",'Detalle del Riesgo'!F58)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C14" s="158" t="str">
         <f>IF($A14="","",LEFT('Detalle del Riesgo'!D63,1))</f>
@@ -22052,7 +22137,7 @@
       </c>
       <c r="B15" s="157">
         <f>IF($A15="","",'Detalle del Riesgo'!F84)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C15" s="158" t="str">
         <f>IF($A15="","",LEFT('Detalle del Riesgo'!D89,1))</f>
@@ -22094,7 +22179,7 @@
       </c>
       <c r="B16" s="157">
         <f>IF($A16="","",'Detalle del Riesgo'!F110)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C16" s="158" t="str">
         <f>IF($A16="","",LEFT('Detalle del Riesgo'!D115,1))</f>
@@ -22118,7 +22203,7 @@
       </c>
       <c r="H16" s="158" t="str">
         <f>IF($A16= "","",'Detalle del Riesgo'!F108)</f>
-        <v>Investigar</v>
+        <v>Aceptar</v>
       </c>
       <c r="I16" s="161">
         <f>IF($A16= "","",'Detalle del Riesgo'!C110)</f>
@@ -22136,7 +22221,7 @@
       </c>
       <c r="B17" s="157">
         <f>IF($A17="","",'Detalle del Riesgo'!F136)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C17" s="158" t="str">
         <f>IF($A17="","",LEFT('Detalle del Riesgo'!D141,1))</f>
@@ -22178,7 +22263,7 @@
       </c>
       <c r="B18" s="157">
         <f>IF($A18="","",'Detalle del Riesgo'!F162)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C18" s="158" t="str">
         <f>IF($A18="","",LEFT('Detalle del Riesgo'!D167,1))</f>
@@ -22202,7 +22287,7 @@
       </c>
       <c r="H18" s="158" t="str">
         <f>IF($A18= "","",'Detalle del Riesgo'!F160)</f>
-        <v>Aceptar</v>
+        <v>Retirar</v>
       </c>
       <c r="I18" s="161">
         <f>IF($A18= "","",'Detalle del Riesgo'!C162)</f>
@@ -22262,7 +22347,7 @@
       </c>
       <c r="B20" s="157">
         <f>IF($A20="","",'Detalle del Riesgo'!F214)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C20" s="158" t="str">
         <f>IF($A20="","",LEFT('Detalle del Riesgo'!D219,1))</f>
@@ -22286,7 +22371,7 @@
       </c>
       <c r="H20" s="158" t="str">
         <f>IF($A20= "","",'Detalle del Riesgo'!F212)</f>
-        <v>Investigar</v>
+        <v>Aceptar</v>
       </c>
       <c r="I20" s="161">
         <f>IF($A20= "","",'Detalle del Riesgo'!C214)</f>
@@ -22304,7 +22389,7 @@
       </c>
       <c r="B21" s="157">
         <f>IF($A21="","",'Detalle del Riesgo'!F240)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C21" s="158" t="str">
         <f>IF($A21="","",LEFT('Detalle del Riesgo'!D245,1))</f>
@@ -22346,7 +22431,7 @@
       </c>
       <c r="B22" s="157">
         <f>IF($A22="","",'Detalle del Riesgo'!F266)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C22" s="158" t="str">
         <f>IF($A22="","",LEFT('Detalle del Riesgo'!D271,1))</f>
@@ -22430,7 +22515,7 @@
       </c>
       <c r="B24" s="157">
         <f>IF($A24="","",'Detalle del Riesgo'!F318)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C24" s="158" t="str">
         <f>IF($A24="","",LEFT('Detalle del Riesgo'!D323,1))</f>
@@ -22454,7 +22539,7 @@
       </c>
       <c r="H24" s="158" t="str">
         <f>IF($A24= "","",'Detalle del Riesgo'!F316)</f>
-        <v>Aceptar</v>
+        <v>Prevenir</v>
       </c>
       <c r="I24" s="161">
         <f>IF($A24= "","",'Detalle del Riesgo'!C318)</f>
@@ -22496,7 +22581,7 @@
       </c>
       <c r="H25" s="158" t="str">
         <f>IF($A25= "","",'Detalle del Riesgo'!F342)</f>
-        <v>Prevenir</v>
+        <v>Mitigar</v>
       </c>
       <c r="I25" s="161">
         <f>IF($A25= "","",'Detalle del Riesgo'!C344)</f>
@@ -22514,7 +22599,7 @@
       </c>
       <c r="B26" s="157">
         <f>IF($A26="","",'Detalle del Riesgo'!F370)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C26" s="158" t="str">
         <f>IF($A26="","",LEFT('Detalle del Riesgo'!D375,1))</f>
@@ -22556,7 +22641,7 @@
       </c>
       <c r="B27" s="157">
         <f>IF($A27="","",'Detalle del Riesgo'!F396)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C27" s="158" t="str">
         <f>IF($A27="","",LEFT('Detalle del Riesgo'!D401,1))</f>
@@ -22598,7 +22683,7 @@
       </c>
       <c r="B28" s="157">
         <f>IF($A28="","",'Detalle del Riesgo'!F422)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" s="158" t="str">
         <f>IF($A28="","",LEFT('Detalle del Riesgo'!D427,1))</f>
@@ -22622,7 +22707,7 @@
       </c>
       <c r="H28" s="158" t="str">
         <f>IF($A28= "","",'Detalle del Riesgo'!F420)</f>
-        <v>Investigar</v>
+        <v>Prevenir</v>
       </c>
       <c r="I28" s="161">
         <f>IF($A28= "","",'Detalle del Riesgo'!C422)</f>
@@ -22640,7 +22725,7 @@
       </c>
       <c r="B29" s="157">
         <f>IF($A29="","",'Detalle del Riesgo'!F448)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C29" s="158" t="str">
         <f>IF($A29="","",LEFT('Detalle del Riesgo'!D453,1))</f>
@@ -22682,7 +22767,7 @@
       </c>
       <c r="B30" s="157">
         <f>IF($A30="","",'Detalle del Riesgo'!F474)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" s="158" t="str">
         <f>IF($A30="","",LEFT('Detalle del Riesgo'!D479,1))</f>
@@ -22724,7 +22809,7 @@
       </c>
       <c r="B31" s="157">
         <f>IF($A31="","",'Detalle del Riesgo'!F500)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" s="158" t="str">
         <f>IF($A31="","",LEFT('Detalle del Riesgo'!D505,1))</f>
@@ -22766,7 +22851,7 @@
       </c>
       <c r="B32" s="157">
         <f>IF($A32="","",'Detalle del Riesgo'!F526)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C32" s="158" t="str">
         <f>IF($A32="","",LEFT('Detalle del Riesgo'!D531,1))</f>
@@ -22808,7 +22893,7 @@
       </c>
       <c r="B33" s="157">
         <f>IF($A33="","",'Detalle del Riesgo'!F552)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C33" s="158" t="str">
         <f>IF($A33="","",LEFT('Detalle del Riesgo'!D557,1))</f>
@@ -23208,7 +23293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:H1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -23221,32 +23306,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="228"/>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
+      <c r="A2" s="237"/>
+      <c r="B2" s="237"/>
+      <c r="C2" s="237"/>
+      <c r="D2" s="237"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="228"/>
-      <c r="B3" s="228"/>
-      <c r="C3" s="228"/>
-      <c r="D3" s="228"/>
+      <c r="A3" s="237"/>
+      <c r="B3" s="237"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="228"/>
-      <c r="B4" s="228"/>
-      <c r="C4" s="228"/>
-      <c r="D4" s="228"/>
+      <c r="A4" s="237"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="237"/>
+      <c r="D4" s="237"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="228"/>
-      <c r="B5" s="228"/>
-      <c r="C5" s="228"/>
-      <c r="D5" s="228"/>
+      <c r="A5" s="237"/>
+      <c r="B5" s="237"/>
+      <c r="C5" s="237"/>
+      <c r="D5" s="237"/>
     </row>
     <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="200" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -23258,13 +23343,13 @@
         <v>120</v>
       </c>
       <c r="D11" s="125" t="s">
+        <v>234</v>
+      </c>
+      <c r="E11" s="121" t="s">
         <v>235</v>
       </c>
-      <c r="E11" s="121" t="s">
+      <c r="F11" s="121" t="s">
         <v>236</v>
-      </c>
-      <c r="F11" s="121" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -23298,7 +23383,7 @@
       </c>
       <c r="D13" s="123">
         <f>Resumen!I7</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" s="123">
         <f>COUNTIF($H$14:$H$1002,"YMitigar")</f>
@@ -23309,7 +23394,7 @@
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -23326,7 +23411,7 @@
       </c>
       <c r="E14" s="124">
         <f>COUNTIF($H$14:$H$1002,"gMitigar")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" s="124">
         <f>COUNTIF($H$14:$H$1002,"GAceptar")</f>
@@ -23347,11 +23432,11 @@
       </c>
       <c r="D15" s="203">
         <f>SUM(D12:D14)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" s="203">
         <f>SUM(E12:E14)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F15" s="203">
         <f>SUM(F12:F14)</f>
@@ -23377,7 +23462,7 @@
     <row r="18" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H18" s="201" t="str">
         <f>CONCATENATE(Resumen!F16,Resumen!H16)</f>
-        <v>GInvestigar</v>
+        <v>GAceptar</v>
       </c>
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.2">
@@ -23389,7 +23474,7 @@
     <row r="20" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H20" s="201" t="str">
         <f>CONCATENATE(Resumen!F18,Resumen!H18)</f>
-        <v>YAceptar</v>
+        <v>YRetirar</v>
       </c>
     </row>
     <row r="21" spans="8:8" x14ac:dyDescent="0.2">
@@ -23401,7 +23486,7 @@
     <row r="22" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H22" s="201" t="str">
         <f>CONCATENATE(Resumen!F20,Resumen!H20)</f>
-        <v>YInvestigar</v>
+        <v>YAceptar</v>
       </c>
     </row>
     <row r="23" spans="8:8" x14ac:dyDescent="0.2">
@@ -23425,13 +23510,13 @@
     <row r="26" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H26" s="201" t="str">
         <f>CONCATENATE(Resumen!F24,Resumen!H24)</f>
-        <v>GAceptar</v>
+        <v>GPrevenir</v>
       </c>
     </row>
     <row r="27" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H27" s="201" t="str">
         <f>CONCATENATE(Resumen!F25,Resumen!H25)</f>
-        <v>GPrevenir</v>
+        <v>GMitigar</v>
       </c>
     </row>
     <row r="28" spans="8:8" x14ac:dyDescent="0.2">
@@ -23449,7 +23534,7 @@
     <row r="30" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H30" s="201" t="str">
         <f>CONCATENATE(Resumen!F28,Resumen!H28)</f>
-        <v>GInvestigar</v>
+        <v>GPrevenir</v>
       </c>
     </row>
     <row r="31" spans="8:8" x14ac:dyDescent="0.2">
@@ -29553,11 +29638,11 @@
       </c>
       <c r="E7" s="54">
         <f>COUNTIF($E$16:$E$45,"Y-Retirar")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" s="55">
         <f>COUNTIF($F$16:$F$45,"Y-Abierto")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" s="51"/>
       <c r="H7" s="52"/>
@@ -29724,11 +29809,11 @@
       </c>
       <c r="E11" s="43">
         <f>SUM(E5:E9)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="40">
         <f>SUM(F5:F10)</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" s="50"/>
       <c r="H11" s="50"/>
@@ -30205,7 +30290,7 @@
       </c>
       <c r="E20" s="51" t="str">
         <f>IF($B20="","",CONCATENATE(I20,"-",Resumen!H16))</f>
-        <v>G-Investigar</v>
+        <v>G-Aceptar</v>
       </c>
       <c r="F20" s="51" t="str">
         <f t="shared" si="0"/>
@@ -30361,15 +30446,15 @@
       </c>
       <c r="E22" s="51" t="str">
         <f>IF($B22="","",CONCATENATE(I22,"-",Resumen!H18))</f>
-        <v>Y-Aceptar</v>
+        <v>Y-Retirar</v>
       </c>
       <c r="F22" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>Y-Abierto</v>
+        <v>Y-Cerrado</v>
       </c>
       <c r="G22" s="51" t="str">
         <f>IF(Resumen!H18="Retirar","Cerrado","Abierto")</f>
-        <v>Abierto</v>
+        <v>Cerrado</v>
       </c>
       <c r="H22" s="9" t="str">
         <f>IF($B$16="","",IF(OR(ISBLANK('Detalle del Riesgo'!F167),ISTEXT('Detalle del Riesgo'!F167)),"",IF($H$15-'Detalle del Riesgo'!F167&gt;$H$14,"Not Modified","M")))</f>
@@ -30481,7 +30566,7 @@
       </c>
       <c r="E24" s="51" t="str">
         <f>IF($B24="","",CONCATENATE(I24,"-",Resumen!H20))</f>
-        <v>Y-Investigar</v>
+        <v>Y-Aceptar</v>
       </c>
       <c r="F24" s="51" t="str">
         <f t="shared" si="0"/>
@@ -30721,7 +30806,7 @@
       </c>
       <c r="E28" s="51" t="str">
         <f>IF($B28="","",CONCATENATE(I28,"-",Resumen!H24))</f>
-        <v>G-Aceptar</v>
+        <v>G-Prevenir</v>
       </c>
       <c r="F28" s="51" t="str">
         <f t="shared" si="0"/>
@@ -30781,7 +30866,7 @@
       </c>
       <c r="E29" s="51" t="str">
         <f>IF($B29="","",CONCATENATE(I29,"-",Resumen!H25))</f>
-        <v>G-Prevenir</v>
+        <v>G-Mitigar</v>
       </c>
       <c r="F29" s="51" t="str">
         <f t="shared" si="0"/>
@@ -30931,7 +31016,7 @@
       </c>
       <c r="E32" s="51" t="str">
         <f>IF($B32="","",CONCATENATE(I32,"-",Resumen!H28))</f>
-        <v>G-Investigar</v>
+        <v>G-Prevenir</v>
       </c>
       <c r="F32" s="51" t="str">
         <f t="shared" si="0"/>

</xml_diff>